<commit_message>
Fix exam security loopholes and student re-entry issues
</commit_message>
<xml_diff>
--- a/assets/templates/student_template.xlsx
+++ b/assets/templates/student_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nmims_quiz_app\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4C2CA1-B2CE-4A4E-83BE-04C032B28DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591929ED-3425-4B3C-8830-F0D5564C680D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,14 +66,14 @@
     <t>2025-2028</t>
   </si>
   <si>
-    <t>johndoe001</t>
+    <t>john.doe01@nmims.in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +83,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,13 +113,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,12 +467,15 @@
       <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{38D4B07E-9683-439C-BBE7-17065CB92469}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance reporting, exam security, and UI for bulk upload and quiz
</commit_message>
<xml_diff>
--- a/assets/templates/student_template.xlsx
+++ b/assets/templates/student_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nmims_quiz_app\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591929ED-3425-4B3C-8830-F0D5564C680D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ACDD50-C279-440A-9BA5-650AA39C7CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>full_name</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>john.doe01@nmims.in</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Welcome123</t>
   </si>
 </sst>
 </file>
@@ -401,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -419,7 +425,7 @@
     <col min="8" max="8" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +450,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -469,6 +478,9 @@
       </c>
       <c r="H2" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added specilizations and bulk students specilization selection
</commit_message>
<xml_diff>
--- a/assets/templates/student_template.xlsx
+++ b/assets/templates/student_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nmims_quiz_app\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ACDD50-C279-440A-9BA5-650AA39C7CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B8D31D-7C49-47D7-85F8-A6F66E463296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>full_name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Welcome123</t>
+  </si>
+  <si>
+    <t>specializations</t>
   </si>
 </sst>
 </file>
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -425,7 +428,7 @@
     <col min="8" max="8" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +456,11 @@
       <c r="I1" t="s">
         <v>14</v>
       </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>

</xml_diff>